<commit_message>
se crea rama para desarrollo Marney Se agregó smartFolder de si es 0km o No al script de EmisionAnswer
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor_Answer.xlsx
+++ b/Sura/DataSource - Emision Motor_Answer.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30646B6-CC0C-41C1-B28D-3FBAD51BC322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68135EDA-D17B-49EB-89CD-1E17C88F3E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t>Usuario</t>
   </si>
@@ -184,6 +192,15 @@
   </si>
   <si>
     <t>ABC12SRPR006</t>
+  </si>
+  <si>
+    <t>Es0km</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -534,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,18 +568,18 @@
     <col min="7" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
-    <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" customWidth="1"/>
+    <col min="13" max="14" width="5.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -603,31 +620,34 @@
         <v>7</v>
       </c>
       <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -668,31 +688,34 @@
         <v>2020</v>
       </c>
       <c r="N2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1000000</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>50</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>52</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>51</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -733,31 +756,34 @@
         <v>2021</v>
       </c>
       <c r="N3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>29</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1000000</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>26</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>36</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>40</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>44</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -797,32 +823,32 @@
       <c r="M4">
         <v>2021</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>29</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1000000</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>37</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>41</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>45</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -862,32 +888,32 @@
       <c r="M5">
         <v>2021</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>18</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>29</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1000000</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>26</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>38</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>42</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>46</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -927,68 +953,68 @@
       <c r="M6">
         <v>2021</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>29</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1000000</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>26</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>43</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>47</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="E16" s="1"/>
     </row>

</xml_diff>